<commit_message>
feat: :sparkles: add effective portfolio calculation
add calculation of shares amount based on the closing day value instead of the amount provided by TR
</commit_message>
<xml_diff>
--- a/data/Assets.xlsx
+++ b/data/Assets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks" sheetId="1" state="visible" r:id="rId3"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -38,10 +38,13 @@
     <t xml:space="preserve">Price</t>
   </si>
   <si>
+    <t xml:space="preserve">CalculatedQuantity</t>
+  </si>
+  <si>
     <t xml:space="preserve">Currency</t>
   </si>
   <si>
-    <t xml:space="preserve">QuantityCalculated</t>
+    <t xml:space="preserve">Investment</t>
   </si>
   <si>
     <t xml:space="preserve">AssetName</t>
@@ -108,9 +111,6 @@
   </si>
   <si>
     <t xml:space="preserve">Apple Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investment</t>
   </si>
   <si>
     <t xml:space="preserve">Expiry</t>
@@ -236,8 +236,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -253,23 +257,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -396,422 +388,431 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="1" sqref="B4:H4 F19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="48.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="47.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>45779</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="n">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="n">
         <v>0.346308</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="G2" s="0" t="str">
+      <c r="H2" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B2,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>Google</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>9</v>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>45751</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="n">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>15.243902</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>1000.3</v>
       </c>
-      <c r="G3" s="0" t="str">
+      <c r="H3" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B3,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>Nasdaq</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <f aca="false">SUM($F$2:F1000)</f>
+      <c r="J3" s="1" t="n">
+        <f aca="false">SUM($G$2:G1000)</f>
         <v>6050.3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>45779</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="n">
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>0.73303</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="G4" s="0" t="str">
+      <c r="H4" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B4,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>Nasdaq</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>45663</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="n">
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="n">
         <v>0.3257696</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="G5" s="0" t="str">
+      <c r="H5" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B5,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>45691</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="n">
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="n">
         <v>0.811661</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="G6" s="0" t="str">
+      <c r="H6" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B6,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="3" t="n">
         <v>45719</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="n">
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="n">
         <v>0.82949</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="G7" s="0" t="str">
+      <c r="H7" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B7,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="3" t="n">
         <v>45749</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="n">
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="n">
         <v>0.907803</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="G8" s="0" t="str">
+      <c r="H8" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B8,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="3" t="n">
         <v>45779</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="n">
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>0.94568</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="G9" s="0" t="str">
+      <c r="H9" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B9,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="3" t="n">
         <v>45686</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="4" t="n">
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="n">
         <v>3.927853</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="G10" s="0" t="str">
+      <c r="H10" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B10,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>Xtrackers II EUR Overnight Rate Swap UCITS ETF 1C</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>45686</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="4" t="n">
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="n">
         <v>3.927853</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="G11" s="0" t="str">
+      <c r="H11" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B11,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>Xtrackers II EUR Overnight Rate Swap UCITS ETF 1D</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="3" t="n">
         <v>45763</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="4" t="n">
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="n">
         <v>1.717327</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="G12" s="0" t="str">
+      <c r="H12" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B12,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>iShares Global Water UCITS ETF USD (Dist)</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="3" t="n">
         <v>45705</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="4" t="n">
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="n">
         <v>1.576789</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="G13" s="0" t="str">
+      <c r="H13" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B13,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>iShares Global Water UCITS ETF USD (Dist)</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="3" t="n">
         <v>45733</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="4" t="n">
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="n">
         <v>1.620745</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="G14" s="0" t="str">
+      <c r="H14" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B14,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>iShares Global Water UCITS ETF USD (Dist)</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="3" t="n">
         <v>45663</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="4" t="n">
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="n">
         <v>1.889287</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="G15" s="0" t="str">
+      <c r="H15" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B15,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>iShares Core MSCI World UCITS ETF USD (Acc)</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="3" t="n">
         <v>45779</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="4" t="n">
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="n">
         <v>4.032908</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="G16" s="0" t="str">
+      <c r="H16" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B16,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>Vanguard FTSE All-World UCITS ETF USD Accumulation</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="3" t="n">
         <v>45691</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="4" t="n">
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="n">
         <v>3.631873</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="G17" s="0" t="str">
+      <c r="H17" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B17,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>Vanguard FTSE All-World UCITS ETF USD Accumulation</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="3" t="n">
         <v>45663</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="4" t="n">
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="n">
         <v>0.844772</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="G18" s="0" t="str">
+      <c r="H18" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B18,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>Apple Inc.</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="3" t="n">
         <v>45779</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="4" t="n">
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="n">
         <v>0.272538</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="G19" s="0" t="str">
+      <c r="H19" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B19,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
         <v>Apple Inc.</v>
       </c>
@@ -835,93 +836,93 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B4:H4 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="56.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>18</v>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="str">
+      <c r="A2" s="1" t="str">
         <f aca="false" t="array" ref="A2:A10">_xlfn.UNIQUE(Stocks!B2:B19)</f>
         <v>1GOOGL.MI</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>19</v>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="str">
+      <c r="A3" s="1" t="str">
         <v>NAQ.F</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>20</v>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="str">
+      <c r="A4" s="1" t="str">
         <v>CSSPX.MI</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="str">
+      <c r="A5" s="1" t="str">
         <v>XEON.DE</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>22</v>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="str">
+      <c r="A6" s="1" t="str">
         <v>XEOD.DE</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>23</v>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="str">
+      <c r="A7" s="1" t="str">
         <v>IQQQ.DE</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>24</v>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="str">
+      <c r="A8" s="1" t="str">
         <v>EUNL.DE</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>25</v>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="str">
+      <c r="A9" s="1" t="str">
         <v>VWCE.DE</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>26</v>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="str">
+      <c r="A10" s="1" t="str">
         <v>APC.DE</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>27</v>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -943,106 +944,110 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="B4:H4 I2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="0" t="s">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
+      <c r="A2" s="3" t="n">
         <v>45770</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>913.11</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="3" t="n">
         <v>47149</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="7" t="b">
+      <c r="F2" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <f aca="false">SUM(B2:B1000)</f>
         <v>4413.11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
+      <c r="A3" s="3" t="n">
         <v>45729</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>2500</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="3" t="n">
         <v>52504</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="7" t="b">
+      <c r="F3" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+      <c r="A4" s="3" t="n">
         <v>45722</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="3" t="n">
         <v>47695</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="7" t="b">
+      <c r="F4" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
+      <c r="A5" s="3" t="n">
         <v>45722</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="3" t="n">
         <v>47118</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="7" t="b">
+      <c r="F5" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1065,104 +1070,104 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="1" sqref="B4:H4 G3"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
+      <c r="A2" s="3" t="n">
         <v>45778</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>10.4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
+      <c r="A3" s="3" t="n">
         <v>45748</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>12.05</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <f aca="false">SUM(B2:B1000)</f>
         <v>86.61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+      <c r="A4" s="3" t="n">
         <v>45717</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>16.91</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
+      <c r="A5" s="3" t="n">
         <v>45689</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>19.83</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="n">
+      <c r="A6" s="3" t="n">
         <v>45689</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>19.83</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="n">
+      <c r="A7" s="3" t="n">
         <v>45722</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>7.42</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="n">
+      <c r="A8" s="3" t="n">
         <v>45701</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>0.17</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>27</v>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1183,51 +1188,51 @@
   </sheetPr>
   <dimension ref="B4:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4:H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.18"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <f aca="false">Bonds!I2</f>
         <v>4413.11</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <f aca="false">Stocks!I3</f>
+      <c r="C5" s="1" t="n">
+        <f aca="false">Stocks!J3</f>
         <v>6050.3</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <f aca="false">IntDiv!G3</f>
         <v>86.61</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <f aca="false">B5+C5</f>
         <v>10463.41</v>
       </c>
-      <c r="H5" s="8" t="n">
+      <c r="H5" s="6" t="n">
         <f aca="false">D5/F5</f>
         <v>0.00827741625340114</v>
       </c>

</xml_diff>

<commit_message>
feat(bonds): :tada: add bonds data input
Included data about bonds info and bonds dividend payments
</commit_message>
<xml_diff>
--- a/data/Assets.xlsx
+++ b/data/Assets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks" sheetId="1" state="visible" r:id="rId3"/>
@@ -14,6 +14,9 @@
     <sheet name="IntDiv" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="Summary" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Stocks!$A$1:$H$23</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="54">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -50,39 +53,39 @@
     <t xml:space="preserve">AssetName</t>
   </si>
   <si>
+    <t xml:space="preserve">CSSPX.MI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotalAssets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUNL.DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APC.DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XEON.DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XEOD.DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VWCE.DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IQQQ.DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAQ.F</t>
+  </si>
+  <si>
     <t xml:space="preserve">1GOOGL.MI</t>
   </si>
   <si>
-    <t xml:space="preserve">EUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotalAssets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAQ.F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSSPX.MI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XEON.DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XEOD.DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IQQQ.DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EUNL.DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VWCE.DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APC.DE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Asset Name</t>
   </si>
   <si>
@@ -113,52 +116,79 @@
     <t xml:space="preserve">Apple Inc.</t>
   </si>
   <si>
+    <t xml:space="preserve">WKN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A19387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3LK3C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3LC3Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2YN0A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Dividends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euro Swap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BondType</t>
+  </si>
+  <si>
     <t xml:space="preserve">Expiry</t>
   </si>
   <si>
-    <t xml:space="preserve">TotalReturn</t>
+    <t xml:space="preserve">Face Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupon Redemption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT0005530032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT0005340929</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XS2282095970</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wolkswagen Leasing</t>
   </si>
   <si>
     <t xml:space="preserve">Corporate</t>
   </si>
   <si>
-    <t xml:space="preserve">TotalBond</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WolksVagen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Italy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avis Budget Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Dividends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Euro Swap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bonds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dividends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Investments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dividend Returns</t>
+    <t xml:space="preserve">XS2648489388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avis Budget Finance</t>
   </si>
 </sst>
 </file>
@@ -168,10 +198,10 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="167" formatCode="0.00%"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="167" formatCode="mm/yy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -192,6 +222,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF443205"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -236,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -257,11 +294,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -274,7 +315,88 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF443205"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF443205"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -388,22 +510,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="47.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,28 +547,28 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
-        <v>45779</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>45663</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.346308</v>
+        <v>0.3257696</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="H2" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B2,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
@@ -458,19 +580,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
-        <v>45751</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>45663</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>15.243902</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="C3" s="1" t="n">
+        <v>1.889287</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>1000.3</v>
+        <v>200</v>
       </c>
       <c r="H3" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B3,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
@@ -478,62 +600,62 @@
       </c>
       <c r="J3" s="1" t="n">
         <f aca="false">SUM($G$2:G1000)</f>
-        <v>6050.3</v>
+        <v>6250.3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
-        <v>45779</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>0.73303</v>
-      </c>
-      <c r="F4" s="2" t="s">
+        <v>45663</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.844772</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="H4" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B4,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>Nasdaq</v>
+        <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
-        <v>45663</v>
+        <v>45686</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>0.3257696</v>
-      </c>
-      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>3.927853</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="H5" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B5,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
+        <v>Xtrackers II EUR Overnight Rate Swap UCITS ETF 1C</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
-        <v>45691</v>
+        <v>45686</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>0.811661</v>
-      </c>
-      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>3.927853</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="1" t="n">
@@ -541,18 +663,18 @@
       </c>
       <c r="H6" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B6,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
+        <v>Xtrackers II EUR Overnight Rate Swap UCITS ETF 1D</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
-        <v>45719</v>
+        <v>45691</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.82949</v>
+        <v>0.811661</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>9</v>
@@ -562,20 +684,20 @@
       </c>
       <c r="H7" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B7,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
+        <v>Google</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
-        <v>45749</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>0.907803</v>
-      </c>
-      <c r="F8" s="2" t="s">
+        <v>45691</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>3.631873</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="1" t="n">
@@ -583,41 +705,41 @@
       </c>
       <c r="H8" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B8,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
+        <v>iShares Global Water UCITS ETF USD (Dist)</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
-        <v>45779</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>0.94568</v>
-      </c>
-      <c r="F9" s="2" t="s">
+        <v>45705</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1.576789</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="H9" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B9,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
+        <v>iShares Core MSCI World UCITS ETF USD (Acc)</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
-        <v>45686</v>
+        <v>45719</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>3.927853</v>
-      </c>
-      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0.82949</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="1" t="n">
@@ -625,81 +747,81 @@
       </c>
       <c r="H10" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B10,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>Xtrackers II EUR Overnight Rate Swap UCITS ETF 1C</v>
+        <v>Google</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
-        <v>45686</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>14</v>
+        <v>45733</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>3.927853</v>
+        <v>1.620745</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="H11" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B11,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>Xtrackers II EUR Overnight Rate Swap UCITS ETF 1D</v>
+        <v>iShares Core MSCI World UCITS ETF USD (Acc)</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
-        <v>45763</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>1.717327</v>
-      </c>
-      <c r="F12" s="1" t="s">
+        <v>45749</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>0.907803</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="H12" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B12,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>iShares Global Water UCITS ETF USD (Dist)</v>
+        <v>Google</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
-        <v>45705</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>1.576789</v>
-      </c>
-      <c r="F13" s="1" t="s">
+        <v>45751</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>15.243902</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>100</v>
+        <v>1000.3</v>
       </c>
       <c r="H13" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B13,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>iShares Global Water UCITS ETF USD (Dist)</v>
+        <v>Vanguard FTSE All-World UCITS ETF USD Accumulation</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
-        <v>45733</v>
+        <v>45763</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>1.620745</v>
+        <v>1.717327</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -709,24 +831,27 @@
       </c>
       <c r="H14" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B14,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>iShares Global Water UCITS ETF USD (Dist)</v>
+        <v>iShares Core MSCI World UCITS ETF USD (Acc)</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
-        <v>45663</v>
+        <v>45763</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>1.889287</v>
+        <v>1576292</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>63.65</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H15" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B15,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
@@ -737,38 +862,38 @@
       <c r="A16" s="3" t="n">
         <v>45779</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>4.032908</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>0.346308</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="H16" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B16,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>Vanguard FTSE All-World UCITS ETF USD Accumulation</v>
+        <v>Apple Inc.</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
-        <v>45691</v>
-      </c>
-      <c r="B17" s="1" t="s">
+        <v>45779</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="1" t="n">
-        <v>3.631873</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="C17" s="2" t="n">
+        <v>0.73303</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="H17" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B17,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
@@ -777,23 +902,23 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
-        <v>45663</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>0.844772</v>
-      </c>
-      <c r="F18" s="1" t="s">
+        <v>45779</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>0.94568</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="H18" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B18,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>Apple Inc.</v>
+        <v>Google</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -801,23 +926,96 @@
         <v>45779</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>0.272538</v>
+        <v>4.032908</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="H19" s="1" t="str">
         <f aca="false">_xlfn.XLOOKUP(B19,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
-        <v>Apple Inc.</v>
+        <v>iShares Global Water UCITS ETF USD (Dist)</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="n">
+        <v>45779</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>0.272538</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>183.46</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="H20" s="1" t="str">
+        <f aca="false">_xlfn.XLOOKUP(B20,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
+        <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="n">
+        <v>45793</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="5" t="n">
+        <v>0.264998</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>188.68</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="H21" s="1" t="str">
+        <f aca="false">_xlfn.XLOOKUP(B21,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
+        <v>iShares Core S&amp;P 500 UCITS ETF USD (Acc)</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="n">
+        <v>45793</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>0.6854</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="H22" s="1" t="str">
+        <f aca="false">_xlfn.XLOOKUP(B22,Mappings!$A$2:$A$10,Mappings!$B$2:$B$10)</f>
+        <v>Vanguard FTSE All-World UCITS ETF USD Accumulation</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H23"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -825,6 +1023,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -855,7 +1054,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="str">
         <f aca="false" t="array" ref="A2:A10">_xlfn.UNIQUE(Stocks!B2:B19)</f>
-        <v>1GOOGL.MI</v>
+        <v>CSSPX.MI</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>20</v>
@@ -863,7 +1062,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="str">
-        <v>NAQ.F</v>
+        <v>EUNL.DE</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
@@ -871,7 +1070,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="str">
-        <v>CSSPX.MI</v>
+        <v>APC.DE</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>22</v>
@@ -895,7 +1094,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="str">
-        <v>IQQQ.DE</v>
+        <v>VWCE.DE</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
@@ -903,7 +1102,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="str">
-        <v>EUNL.DE</v>
+        <v>IQQQ.DE</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>26</v>
@@ -911,7 +1110,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="str">
-        <v>VWCE.DE</v>
+        <v>NAQ.F</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>27</v>
@@ -919,7 +1118,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="str">
-        <v>APC.DE</v>
+        <v>1GOOGL.MI</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>28</v>
@@ -941,10 +1140,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -953,102 +1152,674 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B2" s="6" t="n">
+        <v>45809</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
-        <v>45770</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>913.11</v>
-      </c>
-      <c r="C2" s="3" t="n">
+      <c r="B3" s="6" t="n">
+        <v>45869</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>45901</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>45992</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>46034</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>46053</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>46082</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>46174</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>46234</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>46266</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="6" t="n">
+        <v>46357</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="6" t="n">
+        <v>46399</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <v>46418</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>46447</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="6" t="n">
+        <v>46539</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>46599</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>46631</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="6" t="n">
+        <v>46722</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="6" t="n">
+        <v>46764</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="6" t="n">
+        <v>46783</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="6" t="n">
+        <v>46813</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="6" t="n">
+        <v>46905</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="6" t="n">
+        <v>46965</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="6" t="n">
+        <v>46997</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="6" t="n">
+        <v>47088</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="6" t="n">
+        <v>47130</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="6" t="n">
         <v>47149</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <f aca="false">SUM(B2:B1000)</f>
-        <v>4413.11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>45729</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>2500</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>52504</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>45722</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>500</v>
-      </c>
-      <c r="C4" s="3" t="n">
+      <c r="C28" s="1" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="6" t="n">
+        <v>47178</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="6" t="n">
+        <v>47330</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="6" t="n">
+        <v>47362</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="6" t="n">
+        <v>47514</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="6" t="n">
+        <v>47543</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="6" t="n">
         <v>47695</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>45722</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>500</v>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>47118</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C34" s="1" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="6" t="n">
+        <v>47727</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="6" t="n">
+        <v>47908</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="6" t="n">
+        <v>48092</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="6" t="n">
+        <v>48274</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="6" t="n">
+        <v>48458</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="6" t="n">
+        <v>48639</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="6" t="n">
+        <v>48823</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="6" t="n">
+        <v>49004</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="6" t="n">
+        <v>49188</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="6" t="n">
+        <v>49369</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="6" t="n">
+        <v>49553</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="6" t="n">
+        <v>49735</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="6" t="n">
+        <v>49919</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="6" t="n">
+        <v>50100</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" s="6" t="n">
+        <v>50284</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" s="6" t="n">
+        <v>50465</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" s="6" t="n">
+        <v>50649</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" s="6" t="n">
+        <v>50830</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="6" t="n">
+        <v>51014</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="6" t="n">
+        <v>51196</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="6" t="n">
+        <v>51380</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56" s="6" t="n">
+        <v>51561</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B57" s="6" t="n">
+        <v>51745</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B58" s="6" t="n">
+        <v>51926</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B59" s="6" t="n">
+        <v>52110</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" s="6" t="n">
+        <v>52291</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" s="6" t="n">
+        <v>52475</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>55.47</v>
       </c>
     </row>
   </sheetData>
@@ -1083,7 +1854,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,10 +1865,10 @@
         <v>10.4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1108,7 +1879,7 @@
         <v>12.05</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="1" t="n">
         <f aca="false">SUM(B2:B1000)</f>
@@ -1123,7 +1894,7 @@
         <v>16.91</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,7 +1905,7 @@
         <v>19.83</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,7 +1916,7 @@
         <v>19.83</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1156,7 +1927,7 @@
         <v>7.42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,57 +1957,133 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:H5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.18"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>52110</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>47088</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="n">
-        <f aca="false">Bonds!I2</f>
-        <v>4413.11</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <f aca="false">Stocks!J3</f>
-        <v>6050.3</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <f aca="false">IntDiv!G3</f>
-        <v>86.61</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <f aca="false">B5+C5</f>
-        <v>10463.41</v>
-      </c>
-      <c r="H5" s="6" t="n">
-        <f aca="false">D5/F5</f>
-        <v>0.00827741625340114</v>
-      </c>
-    </row>
+      <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>47695</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(bonds): :sparkles: add visualization of bonds distribution
</commit_message>
<xml_diff>
--- a/data/Assets.xlsx
+++ b/data/Assets.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="56">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -149,13 +149,16 @@
     <t xml:space="preserve">ISIN</t>
   </si>
   <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">BondType</t>
   </si>
   <si>
     <t xml:space="preserve">Expiry</t>
   </si>
   <si>
-    <t xml:space="preserve">Face Value</t>
+    <t xml:space="preserve">FaceValue</t>
   </si>
   <si>
     <t xml:space="preserve">Invested</t>
@@ -167,13 +170,16 @@
     <t xml:space="preserve">IT0005530032</t>
   </si>
   <si>
+    <t xml:space="preserve">Italy 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT0005340929</t>
+  </si>
+  <si>
     <t xml:space="preserve">Italy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Government</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT0005340929</t>
   </si>
   <si>
     <t xml:space="preserve">XS2282095970</t>
@@ -513,7 +519,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -842,7 +848,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>1576292</v>
+        <v>1.576292</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>63.65</v>
@@ -1960,11 +1966,12 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.43"/>
@@ -1978,23 +1985,26 @@
       <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2002,13 +2012,13 @@
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>52110</v>
@@ -2016,7 +2026,7 @@
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="H2" s="1" t="n">
         <v>2500</v>
       </c>
     </row>
@@ -2025,13 +2035,13 @@
         <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="E3" s="7" t="n">
         <v>47088</v>
@@ -2039,7 +2049,7 @@
       <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="H3" s="1" t="n">
         <v>500</v>
       </c>
     </row>
@@ -2048,18 +2058,18 @@
         <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="H4" s="1" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -2068,19 +2078,22 @@
         <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="E5" s="6" t="n">
         <v>47695</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>